<commit_message>
Updated Hw to version 1.0.0, updated documentation
</commit_message>
<xml_diff>
--- a/Bill of Materials/BOM.xlsx
+++ b/Bill of Materials/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="8880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6735"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <t>Design Last Modified</t>
   </si>
   <si>
-    <t>domingo, 21 de noviembre de 2021</t>
+    <t>domingo, 13 de febrero de 2022</t>
   </si>
   <si>
     <t>Total Parts In Design</t>
@@ -212,7 +212,7 @@
     <t>CONN-H16</t>
   </si>
   <si>
-    <t>€4,00</t>
+    <t>€4,50</t>
   </si>
   <si>
     <t>PWM</t>
@@ -781,7 +781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1104,7 +1104,7 @@
         <v>10</v>
       </c>
       <c r="J18" s="27">
-        <v>9.4499999999999993</v>
+        <v>9.9499999999999993</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1131,7 +1131,7 @@
         <v>30</v>
       </c>
       <c r="J19" s="28">
-        <v>21.7</v>
+        <v>22.2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>